<commit_message>
Finishing up the analysis
</commit_message>
<xml_diff>
--- a/output/sites/clust_PCs_validity_measures_CN.xlsx
+++ b/output/sites/clust_PCs_validity_measures_CN.xlsx
@@ -404,28 +404,28 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.696</v>
+        <v>0.669</v>
       </c>
       <c r="E2" t="n">
-        <v>1.288</v>
+        <v>1.068</v>
       </c>
       <c r="F2" t="n">
-        <v>1.262</v>
+        <v>0.93</v>
       </c>
       <c r="G2" t="n">
-        <v>0.345</v>
+        <v>0.357</v>
       </c>
       <c r="H2" t="n">
-        <v>2.379</v>
+        <v>2.417</v>
       </c>
       <c r="I2" t="n">
         <v>4</v>
@@ -433,7 +433,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -451,7 +451,7 @@
         <v>1.063</v>
       </c>
       <c r="G3" t="n">
-        <v>0.515</v>
+        <v>0.39</v>
       </c>
       <c r="H3" t="n">
         <v>2.723</v>
@@ -462,30 +462,59 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.974</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.124</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E5" t="n">
         <v>1.1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>1.042</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.532</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="G5" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="H5" t="n">
         <v>3.075</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I5" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>